<commit_message>
expand Reader() error reporting simplify test_io.py make indent_forest work properly with all iterators remove trailing blank lines in indent_forest()
</commit_message>
<xml_diff>
--- a/tests/schema/fixtures/uncaught-error.xlsx
+++ b/tests/schema/fixtures/uncaught-error.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3260" windowWidth="29160" windowHeight="16840" activeTab="1"/>
+    <workbookView xWindow="800" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Root" sheetId="1" r:id="rId1"/>
-    <sheet name="Nodes" sheetId="2" r:id="rId2"/>
+    <sheet name="Tests" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Nodes!$A$1:$D$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Root!$A$1:$B$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tests!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Id</t>
   </si>
@@ -46,15 +46,6 @@
     <t>€</t>
   </si>
   <si>
-    <t>Root</t>
-  </si>
-  <si>
-    <t>Val1</t>
-  </si>
-  <si>
-    <t>Val2</t>
-  </si>
-  <si>
     <t>node_0</t>
   </si>
   <si>
@@ -62,15 +53,44 @@
   </si>
   <si>
     <t>node_2</t>
+  </si>
+  <si>
+    <t>node_3</t>
+  </si>
+  <si>
+    <t>node_4</t>
+  </si>
+  <si>
+    <t>Float1</t>
+  </si>
+  <si>
+    <t>Bool1</t>
+  </si>
+  <si>
+    <t>'</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -109,9 +129,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -120,6 +140,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,11 +448,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="219" zoomScaleNormal="219" zoomScalePageLayoutView="219" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -454,7 +481,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="279" zoomScaleNormal="279" zoomScalePageLayoutView="279" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -465,78 +492,74 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>8</v>
+      <c r="B6" s="5">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D4"/>
+  <autoFilter ref="A1:C4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>